<commit_message>
Added the monthly report
</commit_message>
<xml_diff>
--- a/budgeteer-web-interface/src/main/resources/report-template.xlsx
+++ b/budgeteer-web-interface/src/main/resources/report-template.xlsx
@@ -13,12 +13,12 @@
   </bookViews>
   <sheets>
     <sheet name="Gesamtübersicht" sheetId="2" r:id="rId1"/>
-    <sheet name="Monatsübersicht" sheetId="1" r:id="rId2"/>
+    <sheet name="Monatsübersicht" sheetId="4" r:id="rId2"/>
     <sheet name="Flags" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Gesamtübersicht!$B$3:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Monatsübersicht!$A$3:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Monatsübersicht!$B$3:$J$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,12 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Bruttoumsatz</t>
-  </si>
-  <si>
-    <t>Zeitraum</t>
   </si>
   <si>
     <t>Gesamtsumme</t>
@@ -227,7 +224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -242,19 +239,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -329,9 +313,8 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -343,13 +326,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="5" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="5" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="5" fillId="9" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="9" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -644,159 +626,159 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="19"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="B4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="13" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5">
         <f>SUMIF(J4:J5,"{name}",D4:D5)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <f>SUMIF(J4:J5,"{name}",E4:E5)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f>SUMIF(J4:J5,"{name}",F4:F5)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f>SUMIF(J4:J5,"{name}",G4:G5)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f>SUMIF(J4:J5,"{name}",H4:H5)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9">
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8">
         <f>SUM(D4:D5)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <f>SUM(E4:E5)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <f>SUM(F4:F5)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <f>SUM(G4:G5)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <f>SUM(H4:H5)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="B3:J3"/>
@@ -810,99 +792,169 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I17"/>
+  <dimension ref="A2:J9"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5">
+        <f>SUMIF(J4:J5,"{name}",D4:D5)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <f>SUMIF(J4:J5,"{name}",E4:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <f>SUMIF(J4:J5,"{name}",F4:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <f>SUMIF(J4:J5,"{name}",G4:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <f>SUMIF(J4:J5,"{name}",H4:H5)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E7" s="7" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="9" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8">
+        <f>SUM(D4:D5)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <f>SUM(E4:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <f>SUM(F4:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
+        <f>SUM(G4:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="8">
+        <f>SUM(H4:H5)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:I3"/>
+  <autoFilter ref="B3:J3"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -913,20 +965,20 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="13" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimized imports, removed unnecessary files, fixed build.gradle, Attributes in the TemplateEntity Class are not preinitialized, TemplateRepository in the TemplateService is private, translated the example, fixed an issue that appeared when exporting in production mode
</commit_message>
<xml_diff>
--- a/budgeteer-web-interface/src/main/resources/report-template.xlsx
+++ b/budgeteer-web-interface/src/main/resources/report-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wirz\git\budgeteer\budgeteer-web-interface\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atanasov\eclipse-workspace\budgeteer\budgeteer-web-interface\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Bruttoumsatz</t>
   </si>
@@ -111,6 +111,45 @@
   </si>
   <si>
     <t>Summe {name}</t>
+  </si>
+  <si>
+    <t>Accounting period</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Until</t>
+  </si>
+  <si>
+    <t>Spent net</t>
+  </si>
+  <si>
+    <t>Spent gross</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Remaining budget net</t>
+  </si>
+  <si>
+    <t>Remaining budget gross</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Invoice recipient</t>
+  </si>
+  <si>
+    <t>Sum according to invoice recipient</t>
+  </si>
+  <si>
+    <t>Sum {name}</t>
+  </si>
+  <si>
+    <t>Total sum</t>
   </si>
 </sst>
 </file>
@@ -624,59 +663,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.88671875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B2" s="17"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>13</v>
       </c>
@@ -708,9 +749,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -722,9 +763,9 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -751,9 +792,9 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -798,25 +839,25 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="17"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
@@ -848,7 +889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>13</v>
       </c>
@@ -880,7 +921,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -894,7 +935,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -923,7 +964,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>1</v>
       </c>
@@ -970,9 +1011,9 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>22</v>
       </c>

</xml_diff>